<commit_message>
Adicao Material PDF Multiplataforma + Testes Iniciais Flutter + Banco de Dados NoSQL
</commit_message>
<xml_diff>
--- a/Dev Multiplataforma/atividades_t1_t2/T1.xlsx
+++ b/Dev Multiplataforma/atividades_t1_t2/T1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ARTHUR\OneDrive\Área de Trabalho\2025_semestre_4\Dev Multiplataforma\atividades_t1_t2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5C1961-448E-4D20-B805-151435982EE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9FA8CE5-FE94-4DC6-9E5F-951FA9628CF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10305" yWindow="0" windowWidth="10185" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Página1" sheetId="1" r:id="rId1"/>
@@ -74,18 +74,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -100,7 +94,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -108,58 +102,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -273,6 +220,50 @@
         <scheme val="minor"/>
       </font>
       <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="4" tint="0.59999389629810485"/>
@@ -304,12 +295,12 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{28E92E92-20AB-4DF1-97FC-3DBF8ADC0EFF}" name="Número da questão/Resposta(s)" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{B5AD3015-33D4-4A4E-B667-EEC936E16E48}" name="A" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{9B59E07D-93B9-45D2-AC37-789F7E6C9DAE}" name="B" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{4964BBF7-1835-4BD1-8D1F-440C0A3A8639}" name="C" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{53583834-03ED-4124-AA6C-E6F4759D6E76}" name="D" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{A1ABA246-F5B1-4032-9094-A0442F3ABEAD}" name="E" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{28E92E92-20AB-4DF1-97FC-3DBF8ADC0EFF}" name="Número da questão/Resposta(s)" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{B5AD3015-33D4-4A4E-B667-EEC936E16E48}" name="A" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{9B59E07D-93B9-45D2-AC37-789F7E6C9DAE}" name="B" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{4964BBF7-1835-4BD1-8D1F-440C0A3A8639}" name="C" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{53583834-03ED-4124-AA6C-E6F4759D6E76}" name="D" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{A1ABA246-F5B1-4032-9094-A0442F3ABEAD}" name="E" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -519,7 +510,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H59" sqref="H59"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -595,22 +586,22 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="G3" s="1"/>
@@ -635,7 +626,7 @@
       <c r="Z3" s="1"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>1</v>
       </c>
       <c r="B4" s="1"/>
@@ -667,7 +658,7 @@
       <c r="Z4" s="1"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>2</v>
       </c>
       <c r="B5" s="1"/>
@@ -699,7 +690,7 @@
       <c r="Z5" s="1"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>3</v>
       </c>
       <c r="B6" s="1"/>
@@ -731,7 +722,7 @@
       <c r="Z6" s="1"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -767,7 +758,7 @@
       <c r="Z7" s="1"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <v>5</v>
       </c>
       <c r="B8" s="1"/>
@@ -801,7 +792,7 @@
       <c r="Z8" s="1"/>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+      <c r="A9" s="1">
         <v>6</v>
       </c>
       <c r="B9" s="1"/>
@@ -833,7 +824,7 @@
       <c r="Z9" s="1"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+      <c r="A10" s="1">
         <v>7</v>
       </c>
       <c r="B10" s="1"/>
@@ -867,7 +858,7 @@
       <c r="Z10" s="1"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
+      <c r="A11" s="1">
         <v>8</v>
       </c>
       <c r="B11" s="1"/>
@@ -899,7 +890,7 @@
       <c r="Z11" s="1"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
+      <c r="A12" s="1">
         <v>9</v>
       </c>
       <c r="B12" s="1"/>
@@ -931,7 +922,7 @@
       <c r="Z12" s="1"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
+      <c r="A13" s="1">
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -963,7 +954,7 @@
       <c r="Z13" s="1"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
+      <c r="A14" s="1">
         <v>11</v>
       </c>
       <c r="B14" s="1"/>
@@ -995,7 +986,7 @@
       <c r="Z14" s="1"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
+      <c r="A15" s="1">
         <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1027,7 +1018,7 @@
       <c r="Z15" s="1"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
+      <c r="A16" s="1">
         <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1059,7 +1050,7 @@
       <c r="Z16" s="1"/>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
+      <c r="A17" s="1">
         <v>14</v>
       </c>
       <c r="B17" s="1"/>
@@ -1091,7 +1082,7 @@
       <c r="Z17" s="1"/>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
+      <c r="A18" s="1">
         <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1125,7 +1116,7 @@
       <c r="Z18" s="1"/>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
+      <c r="A19" s="1">
         <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1157,7 +1148,7 @@
       <c r="Z19" s="1"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
+      <c r="A20" s="1">
         <v>17</v>
       </c>
       <c r="B20" s="1"/>
@@ -1189,7 +1180,7 @@
       <c r="Z20" s="1"/>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
+      <c r="A21" s="1">
         <v>18</v>
       </c>
       <c r="B21" s="1"/>
@@ -1221,7 +1212,7 @@
       <c r="Z21" s="1"/>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
+      <c r="A22" s="1">
         <v>19</v>
       </c>
       <c r="B22" s="1"/>
@@ -1253,7 +1244,7 @@
       <c r="Z22" s="1"/>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
+      <c r="A23" s="1">
         <v>20</v>
       </c>
       <c r="B23" s="1"/>
@@ -1285,7 +1276,7 @@
       <c r="Z23" s="1"/>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A24" s="2">
+      <c r="A24" s="1">
         <v>21</v>
       </c>
       <c r="B24" s="1"/>
@@ -1317,7 +1308,7 @@
       <c r="Z24" s="1"/>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A25" s="2">
+      <c r="A25" s="1">
         <v>22</v>
       </c>
       <c r="B25" s="1"/>
@@ -1349,7 +1340,7 @@
       <c r="Z25" s="1"/>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A26" s="2">
+      <c r="A26" s="1">
         <v>23</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -1381,7 +1372,7 @@
       <c r="Z26" s="1"/>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A27" s="2">
+      <c r="A27" s="1">
         <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -1413,7 +1404,7 @@
       <c r="Z27" s="1"/>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A28" s="2">
+      <c r="A28" s="1">
         <v>25</v>
       </c>
       <c r="B28" s="1"/>
@@ -1445,7 +1436,7 @@
       <c r="Z28" s="1"/>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A29" s="2">
+      <c r="A29" s="1">
         <v>26</v>
       </c>
       <c r="B29" s="1"/>
@@ -1477,7 +1468,7 @@
       <c r="Z29" s="1"/>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A30" s="2">
+      <c r="A30" s="1">
         <v>27</v>
       </c>
       <c r="B30" s="1"/>
@@ -1509,7 +1500,7 @@
       <c r="Z30" s="1"/>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A31" s="2">
+      <c r="A31" s="1">
         <v>28</v>
       </c>
       <c r="B31" s="1"/>
@@ -1543,7 +1534,7 @@
       <c r="Z31" s="1"/>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A32" s="2">
+      <c r="A32" s="1">
         <v>29</v>
       </c>
       <c r="B32" s="1"/>
@@ -1575,7 +1566,7 @@
       <c r="Z32" s="1"/>
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A33" s="2">
+      <c r="A33" s="1">
         <v>30</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1607,7 +1598,7 @@
       <c r="Z33" s="1"/>
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A34" s="2">
+      <c r="A34" s="1">
         <v>31</v>
       </c>
       <c r="B34" s="1"/>
@@ -1639,7 +1630,7 @@
       <c r="Z34" s="1"/>
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A35" s="2">
+      <c r="A35" s="1">
         <v>32</v>
       </c>
       <c r="B35" s="1"/>
@@ -1671,7 +1662,7 @@
       <c r="Z35" s="1"/>
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A36" s="2">
+      <c r="A36" s="1">
         <v>33</v>
       </c>
       <c r="B36" s="1"/>
@@ -1703,7 +1694,7 @@
       <c r="Z36" s="1"/>
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A37" s="2">
+      <c r="A37" s="1">
         <v>34</v>
       </c>
       <c r="B37" s="1"/>
@@ -1735,7 +1726,7 @@
       <c r="Z37" s="1"/>
     </row>
     <row r="38" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A38" s="2">
+      <c r="A38" s="1">
         <v>35</v>
       </c>
       <c r="B38" s="1"/>
@@ -1767,7 +1758,7 @@
       <c r="Z38" s="1"/>
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A39" s="2">
+      <c r="A39" s="1">
         <v>36</v>
       </c>
       <c r="B39" s="1"/>
@@ -1799,7 +1790,7 @@
       <c r="Z39" s="1"/>
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A40" s="2">
+      <c r="A40" s="1">
         <v>37</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -1831,7 +1822,7 @@
       <c r="Z40" s="1"/>
     </row>
     <row r="41" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A41" s="2">
+      <c r="A41" s="1">
         <v>38</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -1863,7 +1854,7 @@
       <c r="Z41" s="1"/>
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A42" s="2">
+      <c r="A42" s="1">
         <v>39</v>
       </c>
       <c r="B42" s="1"/>
@@ -1895,7 +1886,7 @@
       <c r="Z42" s="1"/>
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A43" s="2">
+      <c r="A43" s="1">
         <v>40</v>
       </c>
       <c r="B43" s="1"/>
@@ -1927,7 +1918,7 @@
       <c r="Z43" s="1"/>
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A44" s="2">
+      <c r="A44" s="1">
         <v>41</v>
       </c>
       <c r="B44" s="1"/>
@@ -1961,7 +1952,7 @@
       <c r="Z44" s="1"/>
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A45" s="2">
+      <c r="A45" s="1">
         <v>42</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -1993,7 +1984,7 @@
       <c r="Z45" s="1"/>
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A46" s="2">
+      <c r="A46" s="1">
         <v>43</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -2025,7 +2016,7 @@
       <c r="Z46" s="1"/>
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A47" s="2">
+      <c r="A47" s="1">
         <v>44</v>
       </c>
       <c r="B47" s="1"/>
@@ -2057,7 +2048,7 @@
       <c r="Z47" s="1"/>
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A48" s="2">
+      <c r="A48" s="1">
         <v>45</v>
       </c>
       <c r="B48" s="1"/>
@@ -2089,7 +2080,7 @@
       <c r="Z48" s="1"/>
     </row>
     <row r="49" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A49" s="2">
+      <c r="A49" s="1">
         <v>46</v>
       </c>
       <c r="B49" s="1"/>
@@ -2121,7 +2112,7 @@
       <c r="Z49" s="1"/>
     </row>
     <row r="50" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A50" s="2">
+      <c r="A50" s="1">
         <v>47</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -2153,7 +2144,7 @@
       <c r="Z50" s="1"/>
     </row>
     <row r="51" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A51" s="2">
+      <c r="A51" s="1">
         <v>48</v>
       </c>
       <c r="B51" s="1"/>
@@ -2185,7 +2176,7 @@
       <c r="Z51" s="1"/>
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A52" s="2">
+      <c r="A52" s="1">
         <v>49</v>
       </c>
       <c r="B52" s="1"/>
@@ -2217,7 +2208,7 @@
       <c r="Z52" s="1"/>
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A53" s="2">
+      <c r="A53" s="1">
         <v>50</v>
       </c>
       <c r="B53" s="1" t="s">
@@ -2226,7 +2217,7 @@
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>

</xml_diff>